<commit_message>
Compressed Video and updated Github
</commit_message>
<xml_diff>
--- a/GoogleDrive/Team Organisation/Timesheet after Audit 2.xlsx
+++ b/GoogleDrive/Team Organisation/Timesheet after Audit 2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>This timesheet was created following feedback received during Audit 1 (This only includes individual work)</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>Path Loss Algorithm Tuning</t>
+  </si>
+  <si>
+    <t>18/04/2018</t>
+  </si>
+  <si>
+    <t>Report Work - Risk Matrix</t>
+  </si>
+  <si>
+    <t>23/04/2018</t>
+  </si>
+  <si>
+    <t>Communications, GitHub</t>
   </si>
 </sst>
 </file>
@@ -323,7 +335,7 @@
       </c>
       <c r="H7">
         <f>SUMIF(C:C,"WR",E:E)*24</f>
-        <v>5.166666667</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -365,7 +377,7 @@
       </c>
       <c r="H9">
         <f>SUMIF(C:C,"AB",E:E)*24</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10">
@@ -501,16 +513,32 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.020833333333333332</v>
+      </c>
     </row>
     <row r="20">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.034722222222222224</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="5"/>

</xml_diff>